<commit_message>
UIX-214 - No data should be of type float. Zip codes must be string - add candidate_address.zipCode to header_row for testing - add spreadsheet for other edge case testing
</commit_message>
<xml_diff>
--- a/spreadsheet_import_service/tests/test_spreadsheets/test_spreadsheet.xlsx
+++ b/spreadsheet_import_service/tests/test_spreadsheets/test_spreadsheet.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="5780" yWindow="5360" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test_spreadsheet.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="168">
   <si>
     <t>Candidate ID</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t xml:space="preserve">MBA in Management </t>
+  </si>
+  <si>
+    <t> 99577-0727</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1087,6 +1090,9 @@
       <c r="G2" t="s">
         <v>42</v>
       </c>
+      <c r="L2">
+        <v>95118</v>
+      </c>
       <c r="N2" t="s">
         <v>43</v>
       </c>
@@ -1158,6 +1164,9 @@
       <c r="G3" t="s">
         <v>59</v>
       </c>
+      <c r="L3" t="s">
+        <v>167</v>
+      </c>
       <c r="N3" t="s">
         <v>60</v>
       </c>
@@ -1234,6 +1243,9 @@
       </c>
       <c r="G4" t="s">
         <v>74</v>
+      </c>
+      <c r="L4">
+        <v>95148</v>
       </c>
       <c r="N4" t="s">
         <v>75</v>

</xml_diff>